<commit_message>
Update Lautlabor takes dateien
Ergänzung des Screenshots des neuen Parameters und update aller Dateien
</commit_message>
<xml_diff>
--- a/Lautlabor/1 - takes/Register audio files takes.xlsx
+++ b/Lautlabor/1 - takes/Register audio files takes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="158">
   <si>
     <t>take no.</t>
   </si>
@@ -304,9 +304,6 @@
     <t>Parameter (Gathering): Input level constant</t>
   </si>
   <si>
-    <t>wie liegt die Aufnahme vor (.wav, .flac, .mp3, .ogg)</t>
-  </si>
-  <si>
     <t>Staat (in englisch)</t>
   </si>
   <si>
@@ -457,22 +454,40 @@
     <t>lfd. Nr</t>
   </si>
   <si>
-    <t>SLA-0001</t>
-  </si>
-  <si>
-    <t>SLA-0002</t>
-  </si>
-  <si>
-    <t>SLA-0003</t>
-  </si>
-  <si>
-    <t>SLA-0004</t>
-  </si>
-  <si>
     <t>SLA + lfd.No. =&gt; AccessionNumber</t>
   </si>
   <si>
     <t>.mp3</t>
+  </si>
+  <si>
+    <t>SLA-00001</t>
+  </si>
+  <si>
+    <t>SLA-00002</t>
+  </si>
+  <si>
+    <t>SLA-00003</t>
+  </si>
+  <si>
+    <t>SLA-00004</t>
+  </si>
+  <si>
+    <t>microphone wind shield</t>
+  </si>
+  <si>
+    <t>Parameter (Gathering): Microphone-wind shield</t>
+  </si>
+  <si>
+    <t>wurde mit Windschutz gearbeitet oder nicht (nicht immer bekannt)</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>nein</t>
+  </si>
+  <si>
+    <t>wie liegt die Aufnahme (das Digitalisat) vor (.wav, .flac, .mp3, .ogg)</t>
   </si>
 </sst>
 </file>
@@ -1027,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM18"/>
+  <dimension ref="A1:AN18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,42 +1058,42 @@
     <col min="6" max="6" width="15.5703125" style="5" customWidth="1"/>
     <col min="7" max="7" width="13" style="5" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" style="5"/>
-    <col min="11" max="11" width="18.42578125" style="5" customWidth="1"/>
-    <col min="12" max="12" width="22.28515625" style="5"/>
-    <col min="13" max="13" width="26.7109375" style="5"/>
-    <col min="14" max="14" width="30.42578125" style="5"/>
-    <col min="15" max="15" width="21.5703125" style="5" customWidth="1"/>
-    <col min="16" max="16" width="25.140625" style="13" customWidth="1"/>
-    <col min="17" max="17" width="25.42578125" style="13" customWidth="1"/>
-    <col min="18" max="18" width="23.28515625" style="5" customWidth="1"/>
-    <col min="19" max="19" width="20.42578125" style="5"/>
-    <col min="20" max="20" width="24.42578125" style="5" customWidth="1"/>
-    <col min="21" max="21" width="24.5703125" style="5" customWidth="1"/>
-    <col min="22" max="22" width="26.140625" style="5" customWidth="1"/>
-    <col min="23" max="23" width="27.42578125" style="5" customWidth="1"/>
-    <col min="24" max="24" width="26.5703125" style="14" customWidth="1"/>
-    <col min="25" max="25" width="23.140625" style="5" customWidth="1"/>
-    <col min="26" max="26" width="15.5703125" style="5"/>
-    <col min="27" max="27" width="25.7109375" style="5"/>
-    <col min="28" max="28" width="25.140625" style="5"/>
-    <col min="29" max="29" width="16.28515625" style="5" customWidth="1"/>
-    <col min="30" max="30" width="13.7109375" style="5"/>
-    <col min="31" max="31" width="15.85546875" style="5" customWidth="1"/>
-    <col min="32" max="32" width="13.7109375" style="5"/>
-    <col min="33" max="34" width="15.85546875" style="5" customWidth="1"/>
-    <col min="35" max="35" width="18" style="13" customWidth="1"/>
-    <col min="36" max="37" width="24.7109375" style="18" customWidth="1"/>
-    <col min="38" max="38" width="18" style="5" customWidth="1"/>
-    <col min="39" max="39" width="23.28515625" style="5" customWidth="1"/>
-    <col min="40" max="1030" width="13.7109375" style="5"/>
-    <col min="1031" max="16384" width="9.140625" style="5"/>
+    <col min="9" max="10" width="13.5703125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" style="5"/>
+    <col min="12" max="12" width="18.42578125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="22.28515625" style="5"/>
+    <col min="14" max="14" width="26.7109375" style="5"/>
+    <col min="15" max="15" width="30.42578125" style="5"/>
+    <col min="16" max="16" width="21.5703125" style="5" customWidth="1"/>
+    <col min="17" max="17" width="25.140625" style="13" customWidth="1"/>
+    <col min="18" max="18" width="25.42578125" style="13" customWidth="1"/>
+    <col min="19" max="19" width="23.28515625" style="5" customWidth="1"/>
+    <col min="20" max="20" width="20.42578125" style="5"/>
+    <col min="21" max="21" width="24.42578125" style="5" customWidth="1"/>
+    <col min="22" max="22" width="24.5703125" style="5" customWidth="1"/>
+    <col min="23" max="23" width="26.140625" style="5" customWidth="1"/>
+    <col min="24" max="24" width="27.42578125" style="5" customWidth="1"/>
+    <col min="25" max="25" width="26.5703125" style="14" customWidth="1"/>
+    <col min="26" max="26" width="23.140625" style="5" customWidth="1"/>
+    <col min="27" max="27" width="15.5703125" style="5"/>
+    <col min="28" max="28" width="25.7109375" style="5"/>
+    <col min="29" max="29" width="25.140625" style="5"/>
+    <col min="30" max="30" width="16.28515625" style="5" customWidth="1"/>
+    <col min="31" max="31" width="13.7109375" style="5"/>
+    <col min="32" max="32" width="15.85546875" style="5" customWidth="1"/>
+    <col min="33" max="33" width="13.7109375" style="5"/>
+    <col min="34" max="35" width="15.85546875" style="5" customWidth="1"/>
+    <col min="36" max="36" width="18" style="13" customWidth="1"/>
+    <col min="37" max="38" width="24.7109375" style="18" customWidth="1"/>
+    <col min="39" max="39" width="18" style="5" customWidth="1"/>
+    <col min="40" max="40" width="23.28515625" style="5" customWidth="1"/>
+    <col min="41" max="1031" width="13.7109375" style="5"/>
+    <col min="1032" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>71</v>
@@ -1105,97 +1120,100 @@
         <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="L1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AE1" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="AF1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AH1" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="AI1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>115</v>
       </c>
       <c r="AK1" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>105</v>
+        <v>114</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="C2" s="2"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -1216,19 +1234,20 @@
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="4"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
-      <c r="AI2" s="8"/>
-      <c r="AJ2" s="6"/>
+      <c r="AD2" s="1"/>
+      <c r="AJ2" s="8"/>
       <c r="AK2" s="6"/>
+      <c r="AL2" s="6"/>
     </row>
-    <row r="3" spans="1:39" s="28" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" s="28" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D3" s="29" t="s">
         <v>27</v>
@@ -1249,97 +1268,100 @@
         <v>32</v>
       </c>
       <c r="J3" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="K3" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="K3" s="28" t="s">
-        <v>141</v>
-      </c>
       <c r="L3" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="M3" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="28" t="s">
+      <c r="N3" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="28" t="s">
+      <c r="O3" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="O3" s="28" t="s">
+      <c r="P3" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="P3" s="28" t="s">
+      <c r="Q3" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="Q3" s="28" t="s">
+      <c r="R3" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="R3" s="28" t="s">
+      <c r="S3" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="S3" s="28" t="s">
+      <c r="T3" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="T3" s="28" t="s">
+      <c r="U3" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="U3" s="28" t="s">
+      <c r="V3" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="V3" s="28" t="s">
+      <c r="W3" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="W3" s="28" t="s">
+      <c r="X3" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="X3" s="31" t="s">
+      <c r="Y3" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="Y3" s="28" t="s">
+      <c r="Z3" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="Z3" s="28" t="s">
+      <c r="AA3" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="AA3" s="28" t="s">
+      <c r="AB3" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC3" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="AB3" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="AC3" s="28" t="s">
+      <c r="AD3" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="AD3" s="28" t="s">
+      <c r="AE3" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF3" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG3" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="AE3" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="AF3" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="AG3" s="28" t="s">
-        <v>103</v>
-      </c>
       <c r="AH3" s="28" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="AI3" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="AJ3" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="AJ3" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="AK3" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="AL3" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="AK3" s="29" t="s">
-        <v>120</v>
-      </c>
-      <c r="AL3" s="28" t="s">
-        <v>133</v>
-      </c>
       <c r="AM3" s="28" t="s">
-        <v>135</v>
+        <v>132</v>
+      </c>
+      <c r="AN3" s="28" t="s">
+        <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -1363,13 +1385,14 @@
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="4"/>
       <c r="Z4" s="1"/>
-      <c r="AJ4" s="7"/>
+      <c r="AA4" s="1"/>
       <c r="AK4" s="7"/>
+      <c r="AL4" s="7"/>
     </row>
-    <row r="5" spans="1:39" ht="150" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" ht="150" x14ac:dyDescent="0.25">
       <c r="A5" s="33"/>
       <c r="B5" s="7" t="s">
         <v>79</v>
@@ -1387,106 +1410,109 @@
         <v>46</v>
       </c>
       <c r="G5" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="I5" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="M5" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="I5" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="L5" s="8" t="s">
+      <c r="N5" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="O5" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="P5" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="Q5" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="R5" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="Q5" s="8" t="s">
+      <c r="S5" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="T5" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="U5" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="V5" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="W5" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="X5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y5" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="R5" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="S5" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="T5" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="U5" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="V5" s="8" t="s">
+      <c r="Z5" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="AA5" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="AB5" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="W5" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="X5" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="Y5" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="Z5" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="AA5" s="8" t="s">
+      <c r="AC5" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="AB5" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="AC5" s="8" t="s">
+      <c r="AD5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AD5" s="8" t="s">
+      <c r="AE5" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AE5" s="12" t="s">
-        <v>145</v>
-      </c>
       <c r="AF5" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG5" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="AG5" s="12" t="s">
-        <v>144</v>
-      </c>
       <c r="AH5" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="AI5" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="AJ5" s="6" t="s">
-        <v>117</v>
+        <v>143</v>
+      </c>
+      <c r="AI5" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="AJ5" s="8" t="s">
+        <v>108</v>
       </c>
       <c r="AK5" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="AL5" s="5" t="s">
-        <v>134</v>
+        <v>116</v>
+      </c>
+      <c r="AL5" s="6" t="s">
+        <v>120</v>
       </c>
       <c r="AM5" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
+      </c>
+      <c r="AN5" s="5" t="s">
+        <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:39" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="34"/>
       <c r="B6" s="19"/>
       <c r="C6" s="20"/>
@@ -1494,36 +1520,36 @@
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
-      <c r="L6" s="22"/>
       <c r="M6" s="22"/>
-      <c r="P6" s="24"/>
+      <c r="N6" s="22"/>
       <c r="Q6" s="24"/>
-      <c r="U6" s="25"/>
-      <c r="X6" s="26"/>
-      <c r="Y6" s="22"/>
-      <c r="AA6" s="22"/>
-      <c r="AI6" s="24"/>
-      <c r="AJ6" s="20"/>
+      <c r="R6" s="24"/>
+      <c r="V6" s="25"/>
+      <c r="Y6" s="26"/>
+      <c r="Z6" s="22"/>
+      <c r="AB6" s="22"/>
+      <c r="AJ6" s="24"/>
       <c r="AK6" s="20"/>
+      <c r="AL6" s="20"/>
     </row>
-    <row r="7" spans="1:39" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
       <c r="B7" s="19"/>
       <c r="C7" s="20"/>
       <c r="D7" s="19"/>
       <c r="E7" s="21"/>
       <c r="F7" s="21"/>
-      <c r="M7" s="22"/>
-      <c r="P7" s="24"/>
+      <c r="N7" s="22"/>
       <c r="Q7" s="24"/>
-      <c r="X7" s="27"/>
-      <c r="AI7" s="24"/>
-      <c r="AJ7" s="20"/>
+      <c r="R7" s="24"/>
+      <c r="Y7" s="27"/>
+      <c r="AJ7" s="24"/>
       <c r="AK7" s="20"/>
+      <c r="AL7" s="20"/>
     </row>
-    <row r="8" spans="1:39" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>75</v>
@@ -1546,84 +1572,87 @@
       <c r="H8" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="K8" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="K8" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="M8" s="8" t="s">
+      <c r="L8" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="N8" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="N8" s="8" t="s">
+      <c r="O8" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="O8" s="8" t="s">
+      <c r="P8" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="P8" s="8" t="s">
+      <c r="Q8" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="Q8" s="8" t="s">
+      <c r="R8" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="R8" s="8" t="s">
+      <c r="S8" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="S8" s="8" t="s">
+      <c r="T8" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="T8" s="8"/>
       <c r="U8" s="8"/>
-      <c r="V8" s="8" t="s">
+      <c r="V8" s="8"/>
+      <c r="W8" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="W8" s="8" t="s">
+      <c r="X8" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="X8" s="11">
+      <c r="Y8" s="11">
         <v>41135</v>
       </c>
-      <c r="Y8" s="8" t="s">
+      <c r="Z8" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="Z8" s="8" t="s">
+      <c r="AA8" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="AA8" s="8">
+      <c r="AB8" s="8">
         <v>2</v>
       </c>
-      <c r="AB8" s="8" t="s">
+      <c r="AC8" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AC8" s="8" t="s">
+      <c r="AD8" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="AD8" s="5" t="s">
+      <c r="AE8" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AF8" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="AG8" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="AH8" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI8" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AJ8" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="AI8" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="AJ8" s="6">
+      <c r="AK8" s="6">
         <v>96</v>
       </c>
-      <c r="AK8" s="6">
+      <c r="AL8" s="6">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:39" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>76</v>
@@ -1650,77 +1679,80 @@
         <v>50</v>
       </c>
       <c r="J9" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="K9" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="K9" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="M9" s="8" t="s">
+      <c r="L9" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="N9" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="N9" s="8" t="s">
+      <c r="O9" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="O9" s="8" t="s">
+      <c r="P9" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="P9" s="8" t="s">
+      <c r="Q9" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="Q9" s="8">
+      <c r="R9" s="8">
         <v>1</v>
       </c>
-      <c r="R9" s="8" t="s">
+      <c r="S9" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="S9" s="8" t="s">
+      <c r="T9" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="T9" s="8"/>
       <c r="U9" s="8"/>
-      <c r="V9" s="8" t="s">
+      <c r="V9" s="8"/>
+      <c r="W9" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="W9" s="8" t="s">
+      <c r="X9" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="X9" s="11">
+      <c r="Y9" s="11">
         <v>42262</v>
       </c>
-      <c r="AA9" s="8">
+      <c r="AB9" s="8">
         <v>0</v>
       </c>
-      <c r="AB9" s="8" t="s">
+      <c r="AC9" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AC9" s="8" t="s">
+      <c r="AD9" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AD9" s="5" t="s">
+      <c r="AE9" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AF9" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="AG9" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="AH9" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI9" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AJ9" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="AI9" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="AJ9" s="6">
+      <c r="AK9" s="6">
         <v>96</v>
       </c>
-      <c r="AK9" s="6">
+      <c r="AL9" s="6">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:39" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>77</v>
@@ -1735,69 +1767,69 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="G10" s="8"/>
-      <c r="J10" s="8" t="s">
+      <c r="K10" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="K10" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="M10" s="17" t="s">
+      <c r="L10" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="N10" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="O10" s="17" t="s">
+      <c r="P10" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="P10" s="8" t="s">
+      <c r="Q10" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="Q10" s="17">
+      <c r="R10" s="17">
         <v>2</v>
       </c>
-      <c r="R10" s="17" t="s">
+      <c r="S10" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="S10" s="8" t="s">
+      <c r="T10" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="T10" s="8"/>
       <c r="U10" s="8"/>
-      <c r="V10" s="17" t="s">
+      <c r="V10" s="8"/>
+      <c r="W10" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="W10" s="17" t="s">
+      <c r="X10" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="AB10" s="8" t="s">
+      <c r="AC10" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AD10" s="5" t="s">
+      <c r="AE10" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AF10" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="AG10" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="AH10" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI10" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AJ10" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="AI10" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="AJ10" s="6">
+      <c r="AK10" s="6">
         <v>96</v>
       </c>
-      <c r="AK10" s="6">
+      <c r="AL10" s="6">
         <v>24</v>
       </c>
-      <c r="AL10" s="5" t="s">
+      <c r="AM10" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:39" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>77</v>
@@ -1812,109 +1844,112 @@
         <v>0.53125</v>
       </c>
       <c r="G11" s="8"/>
-      <c r="K11" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="P11" s="8" t="s">
+      <c r="L11" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q11" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="R11" s="17" t="s">
+      <c r="S11" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="S11" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="T11" s="8"/>
+      <c r="T11" s="8" t="s">
+        <v>147</v>
+      </c>
       <c r="U11" s="8"/>
-      <c r="V11" s="17" t="s">
+      <c r="V11" s="8"/>
+      <c r="W11" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="W11" s="17" t="s">
+      <c r="X11" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="Y11" s="17" t="s">
+      <c r="Z11" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="AA11" s="17">
+      <c r="AB11" s="17">
         <v>1</v>
       </c>
-      <c r="AB11" s="8" t="s">
+      <c r="AC11" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AD11" s="5" t="s">
+      <c r="AE11" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AF11" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="AG11" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="AH11" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI11" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="AJ11" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="AI11" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="AJ11" s="6">
+      <c r="AK11" s="6">
         <v>96</v>
       </c>
-      <c r="AK11" s="6">
+      <c r="AL11" s="6">
         <v>24</v>
       </c>
-      <c r="AM11" s="5" t="s">
+      <c r="AN11" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="36"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="17"/>
-      <c r="AI12" s="17"/>
-      <c r="AJ12" s="6"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="17"/>
+      <c r="AJ12" s="17"/>
       <c r="AK12" s="6"/>
+      <c r="AL12" s="6"/>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="36"/>
-      <c r="P13" s="8"/>
-      <c r="AI13" s="17"/>
-      <c r="AJ13" s="6"/>
+      <c r="Q13" s="8"/>
+      <c r="AJ13" s="17"/>
       <c r="AK13" s="6"/>
+      <c r="AL13" s="6"/>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
-      <c r="Q14" s="17"/>
-      <c r="AI14" s="17"/>
-      <c r="AJ14" s="6"/>
+      <c r="R14" s="17"/>
+      <c r="AJ14" s="17"/>
       <c r="AK14" s="6"/>
+      <c r="AL14" s="6"/>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" s="36"/>
-      <c r="Q15" s="17"/>
-      <c r="AI15" s="17"/>
-      <c r="AJ15" s="6"/>
+      <c r="R15" s="17"/>
+      <c r="AJ15" s="17"/>
       <c r="AK15" s="6"/>
+      <c r="AL15" s="6"/>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" s="36"/>
-      <c r="Q16" s="17"/>
-      <c r="AJ16" s="6"/>
+      <c r="R16" s="17"/>
       <c r="AK16" s="6"/>
+      <c r="AL16" s="6"/>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" s="36"/>
-      <c r="Q17" s="17"/>
-      <c r="AJ17" s="6"/>
+      <c r="R17" s="17"/>
       <c r="AK17" s="6"/>
+      <c r="AL17" s="6"/>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="R3" r:id="rId1" display="Als Image an Collection Specimen. Vor die Ordner/Dateinamenangabe: 'http://svzfmkvm16/soundlabor/' anfügen"/>
+    <hyperlink ref="S3" r:id="rId1" display="Als Image an Collection Specimen. Vor die Ordner/Dateinamenangabe: 'http://svzfmkvm16/soundlabor/' anfügen"/>
   </hyperlinks>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="75" firstPageNumber="0" orientation="landscape" r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" r:id="rId2"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Calibri,Fett Kursiv"&amp;F&amp;RSeite &amp;P von &amp;N</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>